<commit_message>
Run deeper hypertuning. ish 100 minutes train time.
</commit_message>
<xml_diff>
--- a/results/All variables without tuition with_cv_3.xlsx
+++ b/results/All variables without tuition with_cv_3.xlsx
@@ -67,25 +67,25 @@
     <t>XGBoost</t>
   </si>
   <si>
-    <t>{'max_depth': 5, 'min_samples_split': 2}</t>
-  </si>
-  <si>
-    <t>{'max_features': 'sqrt', 'n_estimators': 100}</t>
-  </si>
-  <si>
-    <t>{'learning_rate': 0.1, 'num_leaves': 100}</t>
-  </si>
-  <si>
-    <t>{'max_depth': 3, 'n_estimators': 50}</t>
-  </si>
-  <si>
-    <t>DecisionTreeClassifier(max_depth=5)</t>
-  </si>
-  <si>
-    <t>RandomForestClassifier()</t>
-  </si>
-  <si>
-    <t>LGBMClassifier(num_leaves=100)</t>
+    <t>{'max_depth': 5, 'min_samples_leaf': 2, 'min_samples_split': 5}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 20, 'min_samples_split': 2, 'n_estimators': 300}</t>
+  </si>
+  <si>
+    <t>{'learning_rate': 0.05, 'n_estimators': 150, 'num_leaves': 31}</t>
+  </si>
+  <si>
+    <t>{'learning_rate': 0.1, 'max_depth': 5, 'n_estimators': 250}</t>
+  </si>
+  <si>
+    <t>DecisionTreeClassifier(max_depth=5, min_samples_leaf=2, min_samples_split=5)</t>
+  </si>
+  <si>
+    <t>RandomForestClassifier(max_depth=20, n_estimators=300)</t>
+  </si>
+  <si>
+    <t>LGBMClassifier(learning_rate=0.05, n_estimators=150)</t>
   </si>
   <si>
     <t>XGBClassifier(base_score=None, booster=None, callbacks=None,
@@ -93,28 +93,28 @@
               colsample_bytree=None, device=None, early_stopping_rounds=None,
               enable_categorical=True, eval_metric=None, feature_types=None,
               gamma=None, grow_policy=None, importance_type=None,
-              interaction_constraints=None, learning_rate=None, max_bin=None,
+              interaction_constraints=None, learning_rate=0.1, max_bin=None,
               max_cat_threshold=None, max_cat_to_onehot=None,
-              max_delta_step=None, max_depth=3, max_leaves=None,
+              max_delta_step=None, max_depth=5, max_leaves=None,
               min_child_weight=None, missing=nan, monotone_constraints=None,
-              multi_strategy=None, n_estimators=50, n_jobs=None,
+              multi_strategy=None, n_estimators=250, n_jobs=None,
               num_parallel_tree=None, random_state=None, ...)</t>
   </si>
   <si>
-    <t>[[217  60]
+    <t>[[220  57]
  [ 33 416]]</t>
   </si>
   <si>
-    <t>[[225  52]
- [ 29 420]]</t>
-  </si>
-  <si>
-    <t>[[235  42]
- [ 25 424]]</t>
-  </si>
-  <si>
-    <t>[[231  46]
- [ 27 422]]</t>
+    <t>[[219  58]
+ [ 26 423]]</t>
+  </si>
+  <si>
+    <t>[[236  41]
+ [ 23 426]]</t>
+  </si>
+  <si>
+    <t>[[232  45]
+ [ 30 419]]</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
         <v>17</v>
       </c>
       <c r="C2">
-        <v>0.8708484417585021</v>
+        <v>0.8701611565351346</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -539,25 +539,25 @@
         <v>416</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H2">
         <v>33</v>
       </c>
       <c r="I2">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="J2">
-        <v>0.8716795610806306</v>
+        <v>0.8757048798997842</v>
       </c>
       <c r="K2">
-        <v>0.871900826446281</v>
+        <v>0.8760330578512396</v>
       </c>
       <c r="L2">
-        <v>0.8704889040717918</v>
+        <v>0.8748397117703904</v>
       </c>
       <c r="M2">
-        <v>1.215276718139648</v>
+        <v>21.08915519714355</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -568,7 +568,7 @@
         <v>18</v>
       </c>
       <c r="C3">
-        <v>0.8949567484299088</v>
+        <v>0.897023343998104</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -577,28 +577,28 @@
         <v>26</v>
       </c>
       <c r="F3">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="G3">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H3">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I3">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="J3">
-        <v>0.8883029119188929</v>
+        <v>0.8849348615582383</v>
       </c>
       <c r="K3">
-        <v>0.8884297520661157</v>
+        <v>0.8842975206611571</v>
       </c>
       <c r="L3">
-        <v>0.8874065611065154</v>
+        <v>0.8827416648025406</v>
       </c>
       <c r="M3">
-        <v>27.80262041091919</v>
+        <v>676.3029205799103</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -609,7 +609,7 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>0.8959947861120987</v>
+        <v>0.8987617016234151</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -618,28 +618,28 @@
         <v>27</v>
       </c>
       <c r="F4">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="G4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J4">
-        <v>0.9075724152294578</v>
+        <v>0.9118207220212281</v>
       </c>
       <c r="K4">
-        <v>0.9077134986225895</v>
+        <v>0.9118457300275482</v>
       </c>
       <c r="L4">
-        <v>0.9071100316202683</v>
+        <v>0.9112316723071997</v>
       </c>
       <c r="M4">
-        <v>9.424013137817383</v>
+        <v>197.9825568199158</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -650,7 +650,7 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>0.8973764664059722</v>
+        <v>0.8970375636923805</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -659,28 +659,28 @@
         <v>28</v>
       </c>
       <c r="F5">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G5">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I5">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J5">
-        <v>0.8992825747582619</v>
+        <v>0.896332209541876</v>
       </c>
       <c r="K5">
-        <v>0.8994490358126722</v>
+        <v>0.8966942148760331</v>
       </c>
       <c r="L5">
-        <v>0.8987052462325993</v>
+        <v>0.8961053739790885</v>
       </c>
       <c r="M5">
-        <v>9.267918825149536</v>
+        <v>263.7599172592163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>